<commit_message>
Added #15 and 16
</commit_message>
<xml_diff>
--- a/Workshop_List.xlsx
+++ b/Workshop_List.xlsx
@@ -542,35 +542,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,7 +879,7 @@
   <dimension ref="B1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -892,18 +892,18 @@
   <sheetData>
     <row r="1" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -1060,11 +1060,11 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
@@ -1114,7 +1114,7 @@
       <c r="B23" s="11">
         <v>13</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1180,10 +1180,10 @@
       <c r="B29" s="11">
         <v>17</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="12" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1191,10 +1191,10 @@
       <c r="B30" s="11">
         <v>18</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1202,10 +1202,10 @@
       <c r="B31" s="11">
         <v>19</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       <c r="B32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D32" s="2" t="s">

</xml_diff>